<commit_message>
added correction factor to ppm and ppb calc, as Sami PeakWalk used 0.5 ng/mL but the actual was 0.47 ng/mL, so caling factor applied
</commit_message>
<xml_diff>
--- a/Outputs/Tables/T3.xlsx
+++ b/Outputs/Tables/T3.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -777,7 +777,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PFAS</t>
+          <t>Per- and Polyfluoroalkyl Substances (PFAS)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Combustion Byproduct (PAH)</t>
+          <t>Combustion Byproduct (Polycyclic Aromatic Hydrocarbon)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2777,7 +2777,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Insecticide/Pesticide (Insect Repellants)</t>
+          <t>Insecticide/Pesticide (Insect Repellents)</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">

</xml_diff>

<commit_message>
changed all superscript symbols in supplement and tables to letters
</commit_message>
<xml_diff>
--- a/Outputs/Tables/T3.xlsx
+++ b/Outputs/Tables/T3.xlsx
@@ -1,433 +1,425 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11229"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/Outputs/Tables/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2357EA5-57E0-C04A-B896-771E5299069A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33140" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 3" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 3" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="136">
-  <si>
-    <t>Chemical Name</t>
-  </si>
-  <si>
-    <t>Usage Class (Type)</t>
-  </si>
-  <si>
-    <t>FTC</t>
-  </si>
-  <si>
-    <t>FV-PTC</t>
-  </si>
-  <si>
-    <t>PTC</t>
-  </si>
-  <si>
-    <t>p-value</t>
-  </si>
-  <si>
-    <t>Ethylan</t>
-  </si>
-  <si>
-    <t>Insecticide/Pesticide (Organochlorine)</t>
-  </si>
-  <si>
-    <t>40%</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>10%</t>
-  </si>
-  <si>
-    <t>0.002</t>
-  </si>
-  <si>
-    <t>o-Cresol</t>
-  </si>
-  <si>
-    <t>Chemical Synthesis Intermediate</t>
-  </si>
-  <si>
-    <t>25%</t>
-  </si>
-  <si>
-    <t>65%</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
-    <t>0.005</t>
-  </si>
-  <si>
-    <t>o-Toluidineᵃ</t>
-  </si>
-  <si>
-    <t>Dye Intermediate</t>
-  </si>
-  <si>
-    <t>-0.56ᵉ</t>
-  </si>
-  <si>
-    <t>0.30ᵈ</t>
-  </si>
-  <si>
-    <t>0.26ᵈ</t>
-  </si>
-  <si>
-    <t>0.007</t>
-  </si>
-  <si>
-    <t>3-Hydroxycarbofuran</t>
-  </si>
-  <si>
-    <t>Insecticide/Pesticide (Carbamate)</t>
-  </si>
-  <si>
-    <t>55%</t>
-  </si>
-  <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>DNOPᵇ</t>
-  </si>
-  <si>
-    <t>Plasticizer</t>
-  </si>
-  <si>
-    <t>-0.25ᵈ</t>
-  </si>
-  <si>
-    <t>-0.30ᵈ</t>
-  </si>
-  <si>
-    <t>0.56ᵉ</t>
-  </si>
-  <si>
-    <t>0.008</t>
-  </si>
-  <si>
-    <t>2,4-Dimethylphenol</t>
-  </si>
-  <si>
-    <t>-0.36ᵉ</t>
-  </si>
-  <si>
-    <t>0.54ᵈ</t>
-  </si>
-  <si>
-    <t>-0.18ᵉ</t>
-  </si>
-  <si>
-    <t>0.009</t>
-  </si>
-  <si>
-    <t>MEHPᵇ</t>
-  </si>
-  <si>
-    <t>Plasticizer Metabolite</t>
-  </si>
-  <si>
-    <t>0.06ᵈᵉ</t>
-  </si>
-  <si>
-    <t>0.44ᵈ</t>
-  </si>
-  <si>
-    <t>-0.50ᵉ</t>
-  </si>
-  <si>
-    <t>Acetophenone</t>
-  </si>
-  <si>
-    <t>Flavoring or Fragrance Agent</t>
-  </si>
-  <si>
-    <t>85%</t>
-  </si>
-  <si>
-    <t>0.011</t>
-  </si>
-  <si>
-    <t>Fluorantheneᵇ</t>
-  </si>
-  <si>
-    <t>Combustion Byproduct (PAH)</t>
-  </si>
-  <si>
-    <t>-0.34ᵉ</t>
-  </si>
-  <si>
-    <t>-0.18ᵈᵉ</t>
-  </si>
-  <si>
-    <t>0.52ᵈ</t>
-  </si>
-  <si>
-    <t>0.012</t>
-  </si>
-  <si>
-    <t>Menthoneᶜ</t>
-  </si>
-  <si>
-    <t>-0.40ᵉ</t>
-  </si>
-  <si>
-    <t>-0.10ᵈᵉ</t>
-  </si>
-  <si>
-    <t>0.49ᵈ</t>
-  </si>
-  <si>
-    <t>0.014</t>
-  </si>
-  <si>
-    <t>Pyrene</t>
-  </si>
-  <si>
-    <t>-0.09ᵈᵉ</t>
-  </si>
-  <si>
-    <t>-0.38ᵈ</t>
-  </si>
-  <si>
-    <t>0.47ᵉ</t>
-  </si>
-  <si>
-    <t>0.022</t>
-  </si>
-  <si>
-    <t>Methoxychlorᵃᵇ</t>
-  </si>
-  <si>
-    <t>90%</t>
-  </si>
-  <si>
-    <t>0.023</t>
-  </si>
-  <si>
-    <t>TTBNPᵇ</t>
-  </si>
-  <si>
-    <t>Flame Retardant (Brominated)</t>
-  </si>
-  <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>35%</t>
-  </si>
-  <si>
-    <t>0.026</t>
-  </si>
-  <si>
-    <t>Ethyl butyrate</t>
-  </si>
-  <si>
-    <t>0.48ᵉ</t>
-  </si>
-  <si>
-    <t>-0.19ᵈᵉ</t>
-  </si>
-  <si>
-    <t>-0.29ᵈ</t>
-  </si>
-  <si>
-    <t>0.027</t>
-  </si>
-  <si>
-    <t>Benz(a)anthraceneᵃᵇ</t>
-  </si>
-  <si>
-    <t>-0.30ᵉ</t>
-  </si>
-  <si>
-    <t>-0.17ᵈᵉ</t>
-  </si>
-  <si>
-    <t>0.48ᵈ</t>
-  </si>
-  <si>
-    <t>0.028</t>
-  </si>
-  <si>
-    <t>N-MeFOSAAᵃ</t>
-  </si>
-  <si>
-    <t>PFAS</t>
-  </si>
-  <si>
-    <t>0.07ᵈᵉ</t>
-  </si>
-  <si>
-    <t>-0.45ᵈ</t>
-  </si>
-  <si>
-    <t>0.38ᵉ</t>
-  </si>
-  <si>
-    <t>0.029</t>
-  </si>
-  <si>
-    <t>Terbuthylazineᵇ</t>
-  </si>
-  <si>
-    <t>Herbicide (Triazine)</t>
-  </si>
-  <si>
-    <t>MDAᵃᵇᶜ</t>
-  </si>
-  <si>
-    <t>0.030</t>
-  </si>
-  <si>
-    <t>TEEP</t>
-  </si>
-  <si>
-    <t>Insecticide/Pesticide (Organophosphate)</t>
-  </si>
-  <si>
-    <t>0.09ᵈᵉ</t>
-  </si>
-  <si>
-    <t>0.36ᵉ</t>
-  </si>
-  <si>
-    <t>0.031</t>
-  </si>
-  <si>
-    <t>5-NOTᵃ</t>
-  </si>
-  <si>
-    <t>-0.47ᵈ</t>
-  </si>
-  <si>
-    <t>0.21ᵈ</t>
-  </si>
-  <si>
-    <t>0.035</t>
-  </si>
-  <si>
-    <t>Dibutyl phthalateᵇᶜ</t>
-  </si>
-  <si>
-    <t>45%</t>
-  </si>
-  <si>
-    <t>2,4'-Methoxychlor</t>
-  </si>
-  <si>
-    <t>0.036</t>
-  </si>
-  <si>
-    <t>o-aminoazotolueneᵃᵇᶜ</t>
-  </si>
-  <si>
-    <t>0.039</t>
-  </si>
-  <si>
-    <t>OD-PABAᵇ</t>
-  </si>
-  <si>
-    <t>Organic UV Filter</t>
-  </si>
-  <si>
-    <t>Prosulfuronᵇ</t>
-  </si>
-  <si>
-    <t>Herbicide (Sulfonylurea)</t>
-  </si>
-  <si>
-    <t>-0.28ᵉ</t>
-  </si>
-  <si>
-    <t>0.46ᵈ</t>
-  </si>
-  <si>
-    <t>DEET</t>
-  </si>
-  <si>
-    <t>Insecticide/Pesticide (Insect Repellent)</t>
-  </si>
-  <si>
-    <t>-0.46ᵈ</t>
-  </si>
-  <si>
-    <t>0.23ᵈ</t>
-  </si>
-  <si>
-    <t>Hexanoic acid</t>
-  </si>
-  <si>
-    <t>0.042</t>
-  </si>
-  <si>
-    <t>Metalaxylᵇ</t>
-  </si>
-  <si>
-    <t>Fungicide (Other)</t>
-  </si>
-  <si>
-    <t>60%</t>
-  </si>
-  <si>
-    <t>80%</t>
-  </si>
-  <si>
-    <t>Flucythrinate</t>
-  </si>
-  <si>
-    <t>Insecticide/Pesticide (Pyrethroid)</t>
-  </si>
-  <si>
-    <t>-0.24ᵈ</t>
-  </si>
-  <si>
-    <t>-0.21ᵈ</t>
-  </si>
-  <si>
-    <t>0.45ᵈ</t>
-  </si>
-  <si>
-    <t>0.046</t>
-  </si>
-  <si>
-    <t>Anthraceneᵃ</t>
-  </si>
-  <si>
-    <t>0.10ᵈᵉ</t>
-  </si>
-  <si>
-    <t>0.32ᵈ</t>
-  </si>
-  <si>
-    <t>-0.43ᵉ</t>
-  </si>
-  <si>
-    <t>0.049</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ᵃ Possible, likely, or known carcinogen
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+  <si>
+    <t xml:space="preserve">Chemical Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage Class (Type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FV-PTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethylan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insecticide/Pesticide (Organochlorine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o-Cresol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Synthesis Intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o-Toluidineᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dye Intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.56ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-Hydroxycarbofuran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insecticide/Pesticide (Carbamate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNOPᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasticizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.25ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.30ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.56ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4-Dimethylphenol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.36ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.54ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.18ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEHPᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasticizer Metabolite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.50ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetophenone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavoring or Fragrance Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluorantheneᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combustion Byproduct (PAH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.34ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.18ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menthoneᶜ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.40ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.10ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.49ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.09ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.38ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.47ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methoxychlorᵃᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTBNPᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flame Retardant (Brominated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethyl butyrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.19ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.29ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benz(a)anthraceneᵃᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.30ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.17ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-MeFOSAAᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.45ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.38ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terbuthylazineᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbicide (Triazine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDAᵃᵇᶜ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insecticide/Pesticide (Organophosphate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.36ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-NOTᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.47ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dibutyl phthalateᵇᶜ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4'-Methoxychlor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o-aminoazotolueneᵃᵇᶜ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OD-PABAᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic UV Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prosulfuronᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbicide (Sulfonylurea)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.28ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.46ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insecticide/Pesticide (Insect Repellent)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.46ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.23ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexanoic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metalaxylᵇ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fungicide (Other)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flucythrinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insecticide/Pesticide (Pyrethroid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.24ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.21ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.45ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anthraceneᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10ᵈᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.32ᵈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.43ᵉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.049</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ᵃ Possible, likely, or known carcinogen
 ᵇ Potential endocrine disrupting chemical
 ᶜ Indicates level 2 identification
 Abbreviations: 5-NOT = 5-Nitro-o-toluidine; DEET = N,N-Diethyl-meta-toluamide; DNOP = Di-n-octyl phthalate; MDA = 4,4'-Diaminodiphenylmethane; MEHP = Mono-2-ethylhexyl phthalate; N-MeFOSAA = N-Methylperfluoro-1-octanesulfonamidoacetic acid (linear); OD-PABA = Octyl-dimethyl-p-aminobenzoic acid; PAH = polycyclic aromatic hydrocarbon; TEEP = Tetraethyl ethylenediphosphonate; TTBNP = Tris(tribromoneopentyl); UV = ultraviolet</t>
@@ -437,7 +429,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -456,16 +449,16 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <i/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <i/>
     </font>
     <font>
-      <b/>
       <sz val="7.5"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <b/>
     </font>
   </fonts>
   <fills count="3">
@@ -490,24 +483,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -516,35 +502,26 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -826,39 +803,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="30.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="12.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="12.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="12.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="12.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -878,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -898,7 +878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -918,7 +898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -938,7 +918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -958,7 +938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -978,7 +958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -998,7 +978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -1018,7 +998,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1038,7 +1018,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1058,7 +1038,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1078,7 +1058,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
@@ -1098,7 +1078,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -1118,7 +1098,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -1138,7 +1118,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -1158,7 +1138,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -1178,7 +1158,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -1198,7 +1178,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>90</v>
       </c>
@@ -1218,7 +1198,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>92</v>
       </c>
@@ -1238,7 +1218,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>97</v>
       </c>
@@ -1258,7 +1238,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>101</v>
       </c>
@@ -1278,7 +1258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>103</v>
       </c>
@@ -1298,7 +1278,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>105</v>
       </c>
@@ -1318,7 +1298,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>107</v>
       </c>
@@ -1338,7 +1318,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>109</v>
       </c>
@@ -1358,7 +1338,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>113</v>
       </c>
@@ -1378,7 +1358,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
@@ -1398,7 +1378,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>119</v>
       </c>
@@ -1418,7 +1398,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>123</v>
       </c>
@@ -1438,7 +1418,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>129</v>
       </c>
@@ -1458,7 +1438,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="3" t="s">
         <v>134</v>
       </c>
@@ -1468,21 +1448,21 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+    <row r="33" ht="100" customHeight="1">
+      <c r="A33" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A33:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>